<commit_message>
docs: añade documentos para presentar
</commit_message>
<xml_diff>
--- a/data/Tableros_impresos.xlsx
+++ b/data/Tableros_impresos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3e64e3084cf54c9d/Documentos/Semestre 5/Herramientas II/Bingo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3e64e3084cf54c9d/Documentos/Semestre 5/Herramientas II/Bingo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{F10DCFCE-9DF8-4931-9275-B42E356EBF0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5944A487-1CDD-4AE1-A654-51102AC07E32}"/>
+  <xr:revisionPtr revIDLastSave="120" documentId="13_ncr:1_{F10DCFCE-9DF8-4931-9275-B42E356EBF0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A963EE0A-19CE-4EB3-8607-4BE3835D9518}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E622720B-A1F6-43F1-9D69-CBF036925FF7}"/>
   </bookViews>
@@ -519,6 +519,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -840,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{483267FC-3B48-4EAF-908A-8CF5AED86BA5}">
   <dimension ref="B3:X72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AG9" sqref="AG9"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="AH24" sqref="AH24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.140625" defaultRowHeight="37.5" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>